<commit_message>
Feedback Form scenarios : Contact Name,Editing Contact Name Field
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="NewUser" sheetId="1" r:id="rId1"/>
     <sheet name="SignUp" sheetId="2" r:id="rId2"/>
     <sheet name="Login" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="Feedback" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="61">
   <si>
     <t>Email</t>
   </si>
@@ -140,10 +140,67 @@
     <t>dfgdfghfghS</t>
   </si>
   <si>
-    <t>Email Address</t>
-  </si>
-  <si>
     <t>sdf</t>
+  </si>
+  <si>
+    <t>Contact name</t>
+  </si>
+  <si>
+    <t>Primary role</t>
+  </si>
+  <si>
+    <t>Recognition level</t>
+  </si>
+  <si>
+    <t>contact attributes</t>
+  </si>
+  <si>
+    <t>institution</t>
+  </si>
+  <si>
+    <t>institution type</t>
+  </si>
+  <si>
+    <t>Payer</t>
+  </si>
+  <si>
+    <t>IDS Member</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>time spent</t>
+  </si>
+  <si>
+    <t>What topics were discussed?</t>
+  </si>
+  <si>
+    <t>Nirmalkumar Pant</t>
+  </si>
+  <si>
+    <t>MCO Manager</t>
+  </si>
+  <si>
+    <t>National</t>
+  </si>
+  <si>
+    <t>Cardiology</t>
+  </si>
+  <si>
+    <t>Adventist Health System</t>
+  </si>
+  <si>
+    <t>Academic</t>
+  </si>
+  <si>
+    <t>Florida Hospital</t>
+  </si>
+  <si>
+    <t>10 minutes</t>
+  </si>
+  <si>
+    <t>IDS Input</t>
   </si>
 </sst>
 </file>
@@ -204,11 +261,15 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -663,7 +724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -707,7 +768,7 @@
         <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -766,20 +827,97 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J2" s="5">
+        <v>42857</v>
+      </c>
+      <c r="K2" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed feedback scenarios: Contact attribute,payer check box ,IDS check box,Date picker scenario
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="68">
   <si>
     <t>Email</t>
   </si>
@@ -161,46 +161,67 @@
     <t>institution type</t>
   </si>
   <si>
-    <t>Payer</t>
-  </si>
-  <si>
-    <t>IDS Member</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
     <t>time spent</t>
   </si>
   <si>
     <t>What topics were discussed?</t>
   </si>
   <si>
-    <t>Nirmalkumar Pant</t>
-  </si>
-  <si>
-    <t>MCO Manager</t>
-  </si>
-  <si>
     <t>National</t>
   </si>
   <si>
     <t>Cardiology</t>
   </si>
   <si>
-    <t>Adventist Health System</t>
-  </si>
-  <si>
     <t>Academic</t>
   </si>
   <si>
-    <t>Florida Hospital</t>
-  </si>
-  <si>
     <t>10 minutes</t>
   </si>
   <si>
     <t>IDS Input</t>
+  </si>
+  <si>
+    <t>Medical Director</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>02/05/2017</t>
+  </si>
+  <si>
+    <t>Page Name</t>
+  </si>
+  <si>
+    <t>Feedback</t>
+  </si>
+  <si>
+    <t>Auto Testing 1</t>
+  </si>
+  <si>
+    <t>Auto testing 4</t>
+  </si>
+  <si>
+    <t>AutoTest 5 fo</t>
+  </si>
+  <si>
+    <t>Auto testing 6</t>
+  </si>
+  <si>
+    <t>Auto Testing 4</t>
+  </si>
+  <si>
+    <t>Auto Testing 2</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>payer</t>
+  </si>
+  <si>
+    <t>IDS</t>
   </si>
 </sst>
 </file>
@@ -269,7 +290,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -827,97 +848,143 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.85546875" customWidth="1"/>
+    <col min="10" max="10" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.140625" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
         <v>41</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>42</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>43</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>46</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" t="s">
         <v>47</v>
       </c>
-      <c r="H1" t="s">
+      <c r="M1" t="s">
         <v>48</v>
       </c>
-      <c r="I1" t="s">
-        <v>60</v>
-      </c>
-      <c r="J1" t="s">
-        <v>49</v>
-      </c>
-      <c r="K1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
         <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
         <v>58</v>
       </c>
-      <c r="F2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J3" t="s">
+        <v>64</v>
+      </c>
+      <c r="K3" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="5">
-        <v>42857</v>
-      </c>
-      <c r="K2" t="s">
-        <v>59</v>
+      <c r="L3" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactored Some of the scenarios from feedback form
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="69">
   <si>
     <t>Email</t>
   </si>
@@ -200,15 +200,6 @@
     <t>Auto Testing 1</t>
   </si>
   <si>
-    <t>Auto testing 4</t>
-  </si>
-  <si>
-    <t>AutoTest 5 fo</t>
-  </si>
-  <si>
-    <t>Auto testing 6</t>
-  </si>
-  <si>
     <t>Auto Testing 4</t>
   </si>
   <si>
@@ -222,6 +213,18 @@
   </si>
   <si>
     <t>IDS</t>
+  </si>
+  <si>
+    <t>Nirmal Kumar Pant</t>
+  </si>
+  <si>
+    <t>Auto test ing 11</t>
+  </si>
+  <si>
+    <t>Auto testing 8</t>
+  </si>
+  <si>
+    <t>AutoTest 5we</t>
   </si>
 </sst>
 </file>
@@ -851,7 +854,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -893,10 +896,10 @@
         <v>46</v>
       </c>
       <c r="H1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J1" t="s">
         <v>53</v>
@@ -916,7 +919,7 @@
         <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
         <v>54</v>
@@ -928,19 +931,19 @@
         <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G2" t="s">
         <v>51</v>
       </c>
       <c r="H2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="J2" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>56</v>
@@ -954,7 +957,7 @@
         <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C3" t="s">
         <v>54</v>
@@ -963,7 +966,7 @@
         <v>49</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="F3" t="s">
         <v>59</v>
@@ -972,13 +975,13 @@
         <v>51</v>
       </c>
       <c r="H3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="J3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>56</v>

</xml_diff>